<commit_message>
Limpieza de soluciones generadas por el modelo Codex y cambios adaptados para el modelo GPT Neo
</commit_message>
<xml_diff>
--- a/metrics_codex.xlsx
+++ b/metrics_codex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>entry_point</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>solutions</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>result</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pass@1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>pass@5</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>pass@10</t>
         </is>
       </c>
     </row>
@@ -468,7 +493,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Return a class named RouteDomain where an atributte called file is an input given to the class named filepath</t>
+          <t>Define a class named RouteDomain that has an atributte called file. The attribute called file is equal to an input given to the class. The input given to the class is called filepath.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,12 +505,39 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">["    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = open(filepath, 'r')\n        self.file.seek(0)\n\n    def file_len(self):\n        for i, l in enumerate(self.file):\n            pass\n        return i + 1\n\n    def file_seek(self, line_number):\n        self.file.seek(0)\n        for i, l in enumerate(self.file):\n            if i == line_number:\n                return l\n\n    def file_readline(self):\n        return self.file.readline()\n\n    def file_close(self):\n        self.file.close()\n        return\n\n# Return a class named RouteDomain where an at", "    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_routedomain(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the route domain to a variable\n        route_domain = first_line.split(',')[2]\n        #Return the route domain\n        return route_domain\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Category():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_category(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the category to a variable\n        category = first_line.split(',')[1]\n        #Return the category\n        return category\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Hostname():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_hostname(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the hostname to a variable\n        hostname = first_line.split(',')[0]\n        #Return the hostname\n        return hostname\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass IpAddress():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_ipaddress(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the ipaddress to a variable\n        ipaddress = first_line.split(',')[3]\n        #Return the ipaddress\n        return ipaddress\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Ports():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_ports(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the ports to a variable\n        ports = first_line.split(',')[4]\n        #Return the ports\n        return ports\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Protocol():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_protocol(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the protocol to a variable\n        protocol = first_line.split(',')[5]\n        #Return the protocol\n        return protocol\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Description():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_description(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the description to a variable\n        description = first_line.split(',')[6]\n        #Return the description\n        return description\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Profile():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_profile(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the profile to a variable\n        profile = first_line.split(',')[7]\n        #Return the profile\n        return profile\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Partition():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_partition(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the partition to a variable\n        partition = first_line.split(',')[8]\n        #Return the partition\n        return partition\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Vlan():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_vlan(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the vlan to a variable\n        vlan = first_line.split(',')[9]\n        #Return the vlan\n        return vlan\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass Dnat():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_dnat(self):\n        #Open file and read the first line\n        with open(self.file, 'r') as f:\n            first_line = f.readline()\n        #Split the first line and add the dnat to a variable\n        dnat = first_line.split(',')[10]\n        #Return the dnat\n        return dnat\n\n#Return a class named RouteDomain", "    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_routedomain(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            rd_list = line.split(',')\n            return rd_list\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_routedomain(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            rd_list = line.split(',')\n            return rd_list\n\n#Return a class named VS where an atributte called file is an input given to the class named filepath\n\nclass VS():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_list = line.split(',')\n            return vs_list\n\n#Return a class named VS_Pool where an atributte called file is an input given to the class named filepath\n\nclass VS_Pool():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_pool(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_pool_list = line.split(',')\n            return vs_pool_list\n\n#Return a class named VS_Pool_Members where an atributte called file is an input given to the class named filepath\n\nclass VS_Pool_Members():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_pool_members(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_pool_members_list = line.split(',')\n            return vs_pool_members_list\n\n#Return a class named VS_Profile where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_list = line.split(',')\n            return vs_profile_list\n\n#Return a class named VS_Profile_Persistence where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_Persistence():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_persistence(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_persistence_list = line.split(',')\n            return vs_profile_persistence_list\n\n#Return a class named VS_Profile_Server_SSL where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_Server_SSL():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_server_ssl(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_server_ssl_list = line.split(',')\n            return vs_profile_server_ssl_list\n\n#Return a class named VS_Profile_Client_SSL where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_Client_SSL():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_client_ssl(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_client_ssl_list = line.split(',')\n            return vs_profile_client_ssl_list\n\n#Return a class named VS_Profile_DNS where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_DNS():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_dns(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_dns_list = line.split(',')\n            return vs_profile_dns_list\n\n#Return a class named VS_Profile_Fast_HTTP where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_Fast_HTTP():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_fast_http(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_fast_http_list = line.split(',')\n            return vs_profile_fast_http_list\n\n#Return a class named VS_Profile_WAF where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_WAF():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_waf(self):\n        with open(self.filepath, 'r') as f:\n            line = f.read()\n            vs_profile_waf_list = line.split(',')\n            return vs_profile_waf_list\n\n#Return a class named VS_Profile_HTTP_Redirect where an atributte called file is an input given to the class named filepath\n\nclass VS_Profile_HTTP_Redirect():\n    def __init__(self,filepath):\n        self.filepath = filepath\n\n    def get_vs_profile_http_redirect(self):\n        with open(self.file", '    def __init__(self, filepath):\n        self.file = filepath\n\n#Create a method called read_file that takes the file content and return a list with all the lines in the file.\n#Use the with open() as f: method to open the file in read mode.\n\n#Create a method called get_all_domains that takes the content of the file and return a list with all the domains.\n#Use the read_file method to extract the content of the file.\n#Use the split() method to create a list of the domains.\n\n#Create a method called get_unique_domains that takes the content of the file and return a list with all the unique domains.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the set() method to create a list of unique domains.\n\n#Create a method called get_unique_domains_count that takes the content of the file and return the number of unique domains.\n#Use the get_unique_domains method to extract the list of all the unique domains.\n#Use the len() method to get the number of unique domains.\n\n#Create a method called get_domain_count that takes the content of the file and a domain as a parameter and return the number of times the domain is in the file.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the count() method to count the number of times a domain is in the list.\n\n#Create a method called get_most_common_domain that takes the content of the file and return the most common domain.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the most_common() method to get the most common domain.\n\n#Create a method called get_most_common_domain_count that takes the content of the file and return the number of times the most common domain is in the file.\n#Use the get_most_common_domain method to extract the most common domain.\n#Use the get_domain_count method to count the number of times the most common domain is in the file.\n\n#Create a method called get_unique_domains_percentage that takes the content of the file and return the percentage of unique domains.\n#Use the get_unique_domains_count method to extract the number of unique domains.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the len() method to get the number of all the domains.\n#Use the round() method to round the result.\n\n#Create a method called get_most_common_domain_percentage that takes the content of the file and return the percentage of the most common domain.\n#Use the get_most_common_domain_count method to extract the number of times the most common domain is in the file.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the len() method to get the number of all the domains.\n#Use the round() method to round the result.\n\n#Create a method called get_domain_percentage that takes the content of the file and a domain as a parameter and return the percentage of the domain.\n#Use the get_domain_count method to extract the number of times the domain is in the file.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the len() method to get the number of all the domains.\n#Use the round() method to round the result.\n\n#Create a method called get_top_n_domains that takes the content of the file and a number as a parameter and return the top n domains.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the Counter() method to get the top n domains.\n\n#Create a method called get_top_n_domain_count that takes the content of the file and a number as a parameter and return the number of times the top n domains are in the file.\n#Use the get_top_n_domains method to extract the top n domains.\n#Use the get_domain_count method to count the number of times the domain is in the file.\n\n#Create a method called get_top_n_domain_percentage that takes the content of the file and a number as a parameter and return the percentage of the top n domains.\n#Use the get_top_n_domain_count method to extract the number of times the top n domains are in the file.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the len() method to get the number of all the domains.\n#Use the round() method to round the result.\n\n#Create a method called get_domain_series that takes the content of the file and return a series of domains.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the value_counts() method to get the series of domains.\n\n#Create a method called get_domain_count_series that takes the content of the file and return a series of the number of times each domain is in the file.\n#Use the get_domain_series method to extract the series of domains.\n#Use the get_domain_count method to count the number of times the domain is in the file.\n\n#Create a method called get_domain_percentage_series that takes the content of the file and return a series of the percentage of each domain.\n#Use the get_domain_count_series method to extract the series of the number of times each domain is in the file.\n#Use the get_all_domains method to extract the list of all the domains.\n#Use the len() method to get the number of all the domains.\n#Use the round() method to round the result.\n\n#Create a method called get_domain_percentage_summary that takes the content of the file and return a summary of the percentage of each domain.\n#Use the get_domain_percentage_series method to extract the series of the percentage of each domain.\n#Use the describe() method to get the summary of the percentage of each domain.\n\n#Create a method called get_domain_summary that takes the content of the file and return a summary of each domain.\n#Use the get_domain_series method to extract the series of domains.\n#Use the describe() method to get the summary of each domain.\n\n#Create a method called get_top_n_domain_summary that takes the content of the file and a number as a parameter and return a summary of the top n domains.\n#Use the get_top_', '    def __init__(self, filepath):\n        self.file = filepath\n\n#Return a class named DomainFinder where an atributte called domain is an input given to the class named domain_name\n\nclass DomainFinder():\n    def __init__(self, domain_name):\n        self.domain = domain_name\n\n#Apply the function find_domain_route from the class DomainFinder\n\ndef find_domain_route(self):\n\n#The function find_domain_route will find the route of the input file\n    with open(self.file, \'r\') as f:\n#The with open function will open the filepath given to the class RouteDomain\n        route = f.read()\n#The function read will read the filepath given to the class RouteDomain\n        routes = route.split("\\n")\n#The function split will split the route given to the class RouteDomain \n    for route in routes:\n#The for loop will iterate through the routes\n        domain = route.split("\\t")[1]\n#The function split will split the route given to the class RouteDomain\n        if domain == self.domain:\n#The if condition will check if the domain given to the class DomainFinder is equal to the domain\n            return route\n#If the if condition is True, the function find_domain_route will return the route\n\n    return ""\n#If the if condition is False, the function find_domain_route will return an empty string\n\n#Apply the function find_ip_route from the class DomainFinder\n\ndef find_ip_route(self):\n\n#The function find_ip_route will find the route of the input file\n    with open(self.file, \'r\') as f:\n#The with open function will open the filepath given to the class RouteDomain\n        route = f.read()\n#The function read will read the filepath given to the class RouteDomain\n        routes = route.split("\\n")\n#The function split will split the route given to the class RouteDomain \n    for route in routes:\n#The for loop will iterate through the routes\n        domain = route.split("\\t")[1]\n#The function split will split the route given to the class RouteDomain\n        if domain == self.domain:\n#The if condition will check if the domain given to the class DomainFinder is equal to the domain\n            ip_address = route.split("\\t")[0]\n#The function split will split the route given to the class RouteDomain\n            return ip_address\n#If the if condition is True, the function find_ip_route will return the ip_address\n    return ""\n#If the if condition is False, the function find_ip_route will return an empty string\n\n#Apply the function find_all_domain_routes from the class DomainFinder\n\ndef find_all_domain_routes(self):\n\n#The function find_all_domain_routes will find the route of the input file\n    with open(self.file, \'r\') as f:\n#The with open function will open the filepath given to the class RouteDomain\n        route = f.read()\n#The function read will read the filepath given to the class RouteDomain\n        routes = route.split("\\n")\n#The function split will split the route given to the class RouteDomain \n    all_domain_routes = []\n#The variable all_domain_routes is an empty list\n    for route in routes:\n#The for loop will iterate through the routes\n        domain = route.split("\\t")[1]\n#The function split will split the route given to the class RouteDomain\n        if domain == self.domain:\n#The if condition will check if the domain given to the class DomainFinder is equal to the domain\n            all_domain_routes.append(route)\n#If the if condition is True, the function find_all_domain_routes will append the route to the variable all_domain_routes\n    return all_domain_routes\n#The function find_all_domain_routes will return the variable all_domain_routes\n\n#Apply the function find_all_ip_routes from the class DomainFinder\n\ndef find_all_ip_routes(self):\n\n#The function find_all_ip_routes will find the route of the input file\n    with open(self.file, \'r\') as f:\n#The with open function will open the filepath given to the class RouteDomain\n        route = f.read()\n#The function read will read the filepath given to the class RouteDomain\n        routes = route.split("\\n")\n#The function split will split the route given to the class RouteDomain \n    all_ip_routes = []\n#The variable all_ip_routes is an empty list\n    for route in routes:\n#The for loop will iterate through the routes\n        domain = route.split("\\t")[1]\n#The function split will split the route given to the class RouteDomain\n        if domain == self.domain:\n#The if condition will check if the domain given to the class DomainFinder is equal to the domain\n            ip_address = route.split("\\t")[0]\n#The function split will split the route given to the class RouteDomain\n            all_ip_routes.append(ip_address)\n#If the if condition is True, the function find_all_ip_routes will append the ip_address to the variable all_ip_routes\n    return all_ip_routes\n#The function find_all_ip_routes will return the variable all_ip_routes\n\n#Apply the functions find_domain_route, find_ip_route, find_all_domain_routes and find_all_ip_routes to the class DomainFinder\n\nDomainFinder.find_domain_route = find_domain_route\nDomainFinder.find_ip_route = find_ip_route\nDomainFinder.find_all_domain_routes = find_all_domain_routes\nDomainFinder.find_all_ip_routes = find_all_ip_routes\n\n#Define a variable called route_domain that is equal to the class RouteDomain with the input filepath\n\nroute_domain = RouteDomain(\'/etc/hosts\')\n\n#Define a variable called domain_finder that is equal to the class DomainFinder with the input domain', "    def __init__(self, filepath):\n        self.file = filepath\n        #self.file = 'C:\\\\Users\\\\vitor.oliveira\\\\Desktop\\\\toread\\\\route-domain\\\\route-domain.csv'\n\n    def list_all_domains(self):\n        domain_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                domain_list.append(line.split(',')[0])\n        return domain_list\n\n    def list_all_gws(self):\n        gw_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_list.append(line.split(',')[1])\n        return gw_list\n\n    def list_all_vlans(self):\n        vlan_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                vlan_list.append(line.split(',')[2])\n        return vlan_list\n\n    def list_all_ips(self):\n        ip_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                ip_list.append(line.split(',')[3])\n        return ip_list\n\n    def list_all_routes(self):\n        route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                route_list.append(line.split(',')[4])\n        return route_list\n\n    def list_all_ips_with_routes(self):\n        ip_route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                ip_route_list.append(line.split(',')[3] + line.split(',')[4])\n        return ip_route_list\n\n    def list_all_ips_with_vlans(self):\n        ip_vlan_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                ip_vlan_list.append(line.split(',')[3] + line.split(',')[2])\n        return ip_vlan_list\n\n    def list_all_ips_with_vlans_and_routes(self):\n        ip_vlan_route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                ip_vlan_route_list.append(line.split(',')[3] + line.split(',')[2] + line.split(',')[4])\n        return ip_vlan_route_list\n\n    def list_all_vlans_with_routes(self):\n        vlan_route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                vlan_route_list.append(line.split(',')[2] + line.split(',')[4])\n        return vlan_route_list\n\n    def list_all_vlans_with_routes_and_ips(self):\n        vlan_route_ip_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                vlan_route_ip_list.append(line.split(',')[2] + line.split(',')[4] + line.split(',')[3])\n        return vlan_route_ip_list\n\n    def list_all_gws_with_vlans(self):\n        gw_vlan_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_vlan_list.append(line.split(',')[1] + line.split(',')[2])\n        return gw_vlan_list\n\n    def list_all_gws_with_vlans_and_routes(self):\n        gw_vlan_route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_vlan_route_list.append(line.split(',')[1] + line.split(',')[2] + line.split(',')[4])\n        return gw_vlan_route_list\n\n    def list_all_gws_with_vlans_and_routes_and_ips(self):\n        gw_vlan_route_ip_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_vlan_route_ip_list.append(line.split(',')[1] + line.split(',')[2] + line.split(',')[4] + line.split(',')[3])\n        return gw_vlan_route_ip_list\n\n    def list_all_gws_with_routes(self):\n        gw_route_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_route_list.append(line.split(',')[1] + line.split(',')[4])\n        return gw_route_list\n\n    def list_all_gws_with_routes_and_ips(self):\n        gw_route_ip_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_route_ip_list.append(line.split(',')[1] + line.split(',')[4] + line.split(',')[3])\n        return gw_route_ip_list\n\n    def list_all_gws_with_ips(self):\n        gw_ip_list = []\n        with open(self.file, 'r') as f:\n            for line in f:\n                gw_ip_list.append(line.split(',')[1] + line.split(',')[3])\n        return gw_ip_list\n\n    def list_all_domains_with_gws(self):", '    def __init__(self, filepath):\n        self.filepath = filepath\n\n#Define a function named getroute that will return a list of dicts with the route domains\n\ndef getroute(filepath):\n    with open(filepath, "r") as f:\n        text = f.read()\n        text = re.findall("route-domain\\s[^\\n]*", text)\n        route_domains = []\n        for i in text:\n            route_domains.append({"name": i.split()[1], "id": i.split()[2]})\n        return route_domains\n\n#Print the list of route domains\n\nroute_domains = getroute("bigip.txt")\nprint(route_domains)', '    def __init__(self, filepath):\n        self.file = filepath\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = filepath\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file </t>
+          <t>class RouteDomain()
+        def __init__(self, filepath):
+        self.file = filepath</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[False, True, False, True, True, False, False, True, True, True]</t>
+          <t>test0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>["    def __init__(self, filepath):\n        self.file = filepath\n\n    def read_file(self):\n        file = open(self.file)\n        file_list = file.read().splitlines()\n        return file_list\n\n    def route_domain(self):\n        file_list = self.read_file()\n        route_domain_list = []\n        for line in file_list:\n            line = line.split('\\t')\n            route_domain_list.append(line)\n        return route_domain_list\n\n    def domain_list(self):\n        route_domain_list = self.route_domain()\n        domain_list = []\n        for line in route_domain_list:\n            domain_list.append(line[1])\n        return domain_list\n\n    def route_list(self):\n        route_domain_list = self.route_domain()\n        route_list = []\n        for line in route_domain_list:\n            route_list.append(line[0])\n        return route_list\n\nclass Route():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def read_file(self):\n        file = open(self.file)\n        file_list = file.read().splitlines()\n        return file_list\n\n    def route_list(self):\n        file_list = self.read_file()\n        route_list = []\n        for line in file_list:\n            line = line.split('\\t')\n            route_list.append(line)\n        return route_list\n\n    def domain_list(self):\n        route_list = self.route_list()\n        domain_list = []\n        for line in route_list:\n            domain_list.append(line[1])\n        return domain_list\n\n    def route_list(self):\n        route_list = self.route_list()\n        route_list = []\n        for line in route_list:\n            route_list.append(line[0])\n        return route_list\n\n", '    def __init__(self, filepath):\n        self.file = filepath\n\n    def __str__(self):\n        return "RouteDomain({})".format(self.file)\n\n    def read_file(self):\n        with open(self.file, "r") as f:\n            text = f.readlines()\n            return text\n\n    def parse_domain(self):\n        text = self.read_file()\n        domain = []\n        for line in text:\n            if line.startswith("domain:"):\n                domain.append(line.split(":")[1].strip())\n        return domain\n\n    def parse_route(self):\n        text = self.read_file()\n        route = []\n        for line in text:\n            if line.startswith("route:"):\n                route.append(line.split(":")[1].strip())\n        return route\n\n    def parse_net(self):\n        text = self.read_file()\n        net = []\n        for line in text:\n            if line.startswith("net:"):\n                net.append(line.split(":")[1].strip())\n        return net\n\n    def parse_as(self):\n        text = self.read_file()\n        as_ = []\n        for line in text:\n            if line.startswith("as:"):\n                as_.append(line.split(":")[1].strip())\n        return as_\n\n    def parse_descr(self):\n        text = self.read_file()\n        descr = []\n        for line in text:\n            if line.startswith("descr:"):\n                descr.append(line.split(":")[1].strip())\n        return descr\n\n    def parse_origin(self):\n        text = self.read_file()\n        origin = []\n        for line in text:\n            if line.startswith("origin:"):\n                origin.append(line.split(":")[1].strip())\n        return origin\n\n    def parse_members(self):\n        text = self.read_file()\n        members = []\n        for line in text:\n            if line.startswith("members:"):\n                members.append(line.split(":")[1].strip())\n        return members\n\n    def parse_mnt_lower(self):\n        text = self.read_file()\n        mnt_lower = []\n        for line in text:\n            if line.startswith("mnt-lower:"):\n                mnt_lower.append(line.split(":")[1].strip())\n        return mnt_lower\n\n    def parse_mnt_routes(self):\n        text = self.read_file()\n        mnt_routes = []\n        for line in text:\n            if line.startswith("mnt-routes:"):\n                mnt_routes.append(line.split(":")[1].strip())\n        return mnt_routes\n\n    def parse_mnt_by(self):\n        text = self.read_file()\n        mnt_by = []\n        for line in text:\n            if line.startswith("mnt-by:"):\n                mnt_by.append(line.split(":")[1].strip())\n        return mnt_by\n\n    def parse_changed(self):\n        text = self.read_file()\n        changed = []\n        for line in text:\n            if line.startswith("changed:"):\n                changed.append(line.split(":")[1].strip())\n        return changed\n\n    def parse_source(self):\n        text = self.read_file()\n        source = []\n        for line in text:\n            if line.startswith("source:"):\n                source.append(line.split(":")[1].strip())\n        return source\n\n    def parse_remarks(self):\n        text = self.read_file()\n        remarks = []\n        for line in text:\n            if line.startswith("remarks:"):\n                remarks.append(line.split(":")[1].strip())\n        return remarks\n\n    def parse_notify(self):\n        text = self.read_file()\n        notify = []\n        for line in text:\n            if line.startswith("notify:"):\n                notify.append(line.split(":")[1].strip())\n        return notify\n\n    def parse_org(self):\n        text = self.read_file()\n        org = []\n        for line in text:\n            if line.startswith("org:"):\n                org.append(line.split(":")[1].strip())\n        return org\n\n    def parse_admin_c(self):\n        text = self.read_file()\n        admin_c = []\n        for line in text:\n            if line.startswith("admin-c:"):\n                admin_c.append(line.split(":")[1].strip())\n        return admin_c\n\n', '\ndef __init__(self, filepath):\n\nself.file = filepath\n\n\n', '    def __init__(self, filepath):\n        self.file = filepath\n        \n    def get_file(self):\n        return self.file\n    \n    def get_domain(self):\n        return self.file.split("/")[1]\n    \n    def get_path(self):\n        return self.file.split("/")[0]\n    \n    def get_filename(self):\n        return self.file.split("/")[2]\n    \n    def get_basename(self):\n        return self.file.split("/")[2].split(".")[0]\n    \n    def get_extension(self):\n        return self.file.split("/")[2].split(".")[1]\n    \n    def get_file_path(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1]\n    \n    def get_filename_with_path(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2]\n    \n    def get_filename_without_extension(self):\n        return self.file.split("/")[2].split(".")[0]\n    \n    def get_filename_without_extension_with_path(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2].split(".")[0]\n    \n    def get_filename_without_extension_with_domain(self):\n        return self.file.split("/")[1] + "/" + self.file.split("/")[2].split(".")[0]\n    \n    def get_filename_without_extension_with_path_and_domain(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2].split(".")[0]\n    \n    def get_filename_without_extension_with_path_and_domain_camel_case(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2].split(".")[0].title()\n    \n    def get_filename_with_path_and_domain_camel_case(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2].title()\n    \n    def get_filename_camel_case(self):\n        return self.file.split("/")[2].title()\n    \n    def get_filename_without_extension_camel_case(self):\n        return self.file.split("/")[2].split(".")[0].title()\n    \n    def get_file_path_camel_case(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1].title()\n    \n    def get_file_path_camel_case_without_slash(self):\n        return self.file.split("/")[0] + self.file.split("/")[1].title()\n    \n    def get_file_path_camel_case_without_slash_without_dot(self):\n        return self.file.split("/")[0] + self.file.split("/")[1].title() + "." + self.file.split("/")[2].split(".")[1]\n    \n    def get_file_path_camel_case_without_slash_without_dot_without_extension(self):\n        return self.file.split("/")[0] + self.file.split("/")[1].title()\n    \n    def get_file_path_camel_case_without_slash_without_dot_without_extension_without_dot(self):\n        return self.file.split("/")[0] + self.file.split("/")[1].title() + "."\n    \n    def get_file_path_without_slash(self):\n        return self.file.split("/")[0] + self.file.split("/")[1]\n    \n    def get_file_path_without_slash_without_dot(self):\n        return self.file.split("/")[0] + self.file.split("/")[1] + "." + self.file.split("/")[2].split(".")[1]\n    \n    def get_file_path_without_slash_without_dot_without_extension(self):\n        return self.file.split("/")[0] + self.file.split("/")[1]\n    \n    def get_file_path_without_slash_without_dot_without_extension_without_dot(self):\n        return self.file.split("/")[0] + self.file.split("/")[1] + "."\n    \n    def get_filename_with_path_and_domain_camel_case_without_dot(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1] + "/" + self.file.split("/")[2].title() + "."\n    \n    def get_filename_camel_case_without_dot(self):\n        return self.file.split("/")[2].title() + "."\n    \n    def get_filename_without_extension_camel_case_without_dot(self):\n        return self.file.split("/")[2].split(".")[0].title() + "."\n    \n    def get_file_path_camel_case_without_dot(self):\n        return self.file.split("/")[0] + "/" + self.file.split("/")[1].title() + "."\n    \n    def get_file_path_', "    def __init__(self, filepath):\n        self.file = filepath\n\n\n\n\ndef read_file_to_list(file, list_routes):\n    with open(file, 'r') as f:\n        for line in f:\n            list_routes.append(line)\n    return list_routes\n\n\n\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n\n\ndef route_domains(domains):\n\n    \n    rd_dict = {}\n\n    \n    route_domain = {}\n\n    \n    filepath = 'file'\n\n    \n    rd_obj = RouteDomain(filepath)\n\n    \n    file_name = rd_obj.file\n\n    \n    route_domains = route_domain.file\n\n    \n    file_handler = open(file_name, 'r')\n\n    \n    file_input = file_handler.read()\n\n    \n    lines = file_input.splitlines()\n\n    \n    route_domain_list = rd_dict.keys()\n\n    \n    route_domain_set = route_domain_list.sort()\n\n    \n    route_domain_set = route_domain_list.sort()\n\n    \n    route_domain_dict = route_domain_set.sort()\n\n    \n    rd_dict = route_domain_dict.sort()\n\n    \n    route_domain_list = rd_dict.keys()\n\n    \n    route_domain_set = route_domain_list.sort()\n\n    \n    route_domain_dict = route_domain_set.sort()\n\n    \n    rd_dict = route_domain_dict.sort()\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        #print(self.file)\n        #print(filepath)\n\nclass Node():\n    def __init__(self, name):\n        self.name = name\n        self.neighbours = []\n\nroute = RouteDomain('/Users/adriano/Desktop/Routing_Scripts/route.txt')\n\nnodes = []\n\nnode_names = []\n\nwith open(route.file, 'r') as f:\n    #Read the file line by line.\n    for line in f:\n        #Remove the spaces and the new line character.\n        line = line.strip()\n        #print(line)\n        #Split the line in two parts. The delimiter is a space.\n        line = line.split()\n        #print(line)\n        #The first element of the line is the name of the node.\n        node_name = line[0]\n        #print(node_name)\n        #The second element of the line is the list of neighbours of the node.\n        node_neighbours = line[1:]\n        #print(node_neighbours)\n        #Append the name of the node to the list node_names.\n        node_names.append(node_name)\n        #print(node_names)\n        #Append the list [node_name, node_neighbours] to the list nodes.\n        nodes.append([node_name, node_neighbours])\n        #print(nodes)\n\nnodes_dict = {}\n\nnodes_list = []\n\nall_neighbours = []\n\nfor i in nodes:\n    #print(i)\n    #The name of the node is the first element of the list.\n    node_name = i[0]\n    #print(node_name)\n    #The neighbours of the node are the second element of the list.\n    node_neighbours = i[1]\n    #print(node_neighbours)\n    #Create an object of the class Node called node.\n    node = Node(node_name)\n    #print(node)\n    #print(node.name)\n    #print(node.neighbours)\n    #For each element of the list node_neighbours.\n    for j in node_neighbours:\n        #print(j)\n        #Append the element to the list node.neighbours.\n        node.neighbours.append(j)\n        #print(node.neighbours)\n        #Append the element to the list all_neighbours.\n        all_neighbours.append(j)\n        #print(all_neighbours)\n    #Append the object node to the list nodes_list.\n    nodes_list.append(node)\n    #print(nodes_list)\n    #The key is the name of the node, and the value is the object node.\n    nodes_dict[node_name] = node\n    #print(nodes_dict)\n\nnodes_not_in_neighbours = []\n\nfor i in node_names:\n    #print(i)\n    #If the element is not in the list all_neighbours.\n    if i not in all_neighbours:\n        #Append the element to the list nodes_not_in_neighbours.\n        nodes_not_in_neighbours.append(i)\n        #print(nodes_not_in_neighbours)\n\nnodes_in_neighbours = []\n\nfor i in node_names:\n    #print(i)\n    #If the element is in the list all_neighbours.\n    if i in all_neighbours:\n        #Append the element to the list nodes_in_neighbours.\n        nodes_in_neighbours.append(i)\n        #print(nodes_in_neighbours)\n\nnodes_not_in_nodes = []\n\nfor i in all_neighbours:\n    #print(i)\n    #If the element is not in the list node_names.\n    if i not in node_names:\n        #Append the element to the list nodes_not_in_nodes.\n        nodes_not_in_nodes.append(i)\n        #print(nodes_not_in_nodes)\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n\n\n    def read_file(self):\n        with open(self.file, 'r') as f:\n            data = f.readlines()\n        return data\n\n\n    def check_hosts(self, hostname):\n        data = self.read_file()\n        for line in data:\n            if hostname in line:\n                return line\n\n\n\n    def get_ip(self, hostname):\n        data = self.read_file()\n        for line in data:\n            if hostname in line:\n                ip = line.split()[1]\n                return ip\n\n\n    def get_hostname(self, ip):\n        data = self.read_file()\n        for line in data:\n            if ip in line:\n                hostname = line.split()[0]\n                return hostname\n\n\n    def add_host(self, hostname, ip):\n        data = self.read_file()\n        data.append(hostname + ' ' + ip + '\\n')\n        with open(self.file, 'w') as f:\n            f.writelines(data)\n\n\n    def del_host(self, hostname):\n        data = self.read_file()\n        for line in data:\n            if hostname in line:\n                data.remove(line)\n        with open(self.file, 'w') as f:\n            f.writelines(data)\n\n\n    def update_host(self, hostname, ip):\n        data = self.read_file()\n        for line in data:\n            if hostname in line:\n                data.remove(line)\n                data.append(hostname + ' ' + ip + '\\n')\n        with open(self.file, 'w') as f:\n            f.writelines(data)\n\n\n    def get_all_hosts(self):\n        data = self.read_file()\n        return data\n\n\n    def get_all_hosts_ip(self):\n        data = self.read_file()\n        for line in data:\n            line = line.split()\n            hostname = line[0]\n            ip = line[1]\n            dic = {hostname: ip}\n        return dic", '    def __init__(self, filepath):\n        self.file = filepath\n\n\nclass Domain:\n    def __init__(self, filepath):\n        self.file = filepath\n\n\n', '    def __init__(self, filepath):\n        self.file = filepath\n    filepath = input("Please enter the filepath: ")\n    return filepath\nroute_domain = RouteDomain(filepath)\n    with open(file, \'r\') as file:\n        for line in file:\n            print(line)\nroute_domain.open_file()\n\n\n\nwith open(filepath, \'r\') as file:\n    for line in file:\n        print(line)\n    def __init__(self, filepath):\n        self.filepath = filepath\n\n    def read_file(self):\n        with open(self.filepath, \'r\') as file:\n            for line in file:\n                print(line)\n\nfilepath = input("Please enter the filepath: ")\nroute_domain = RouteDomain(filepath)\nroute_domain.read_file()\n']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[True, True, False, False, True, True, False, True, True, False]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -497,7 +549,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Return a class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.</t>
+          <t>Define a class named RouteDomain that has an atributte called file. The attribute called file is equal to an input given to the class. The input given to the class is called filepath. Obtain the extension of the file. Define a new attribute in the class named file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class. Do not use os or sys libraries</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,12 +561,41 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>["    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        else:\n            print('File format not supported')\n\n#Create a class named FileTXT where an atributte called file is an input given to the class named filepath. Define a new method called read_txtfile that reads the file and returns the number of words in the file.\nclass FileTXT():\n    def __init__(self, filepath):\n        self.file = filepath\n    \n    def read_txtfile(self):\n        file_object = open(self.file, 'r')\n        file_content = file_object.read()\n        file_object.close()\n        return len(file_content.split())\n\n#Create a class named FileCSV where an atributte called file is an input given to the class named filepath. Define a new method called read_csvfile that reads the file and returns the number of rows in the file.\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n    \n    def read_csvfile(self):\n        import csv\n        file_object = open(self.file, 'r')\n        file_content = csv.reader(file_object)\n        file_object.close()\n        return len(list(file_content))\n#Instantiate the RouteDomain class with a file that has the extension csv.\nroute_domain = RouteDomain('test.csv')\n#Print the instance of the class.\nprint(route_domain)\n\n#Print the file_entity attribute of the instance.\nprint(route_domain.file_entity)\n\n#Print the file_extension attribute of the instance.\nprint(route_domain.file_extension)\n\n#Instantiate the RouteDomain class with a file that has the extension txt.\nroute_domain = RouteDomain('test.txt')\n#Print the instance of the class.\nprint(route_domain)\n\n#Print the file_entity attribute of the instance.\nprint(route_domain.file_entity)\n\n#Print the file_extension attribute of the instance.\nprint(route_domain.file_extension)\n\n#Create a file named test.csv and save it in the current directory.\nimport csv\nfile_object = open('test.csv', 'w')\nfile_content = csv.writer(file_object)\nfile_content.writerow(['Name', 'Age', 'Job'])\nfile_content.writerow(['Luis', 24, 'Data Scientist'])\nfile_content.writerow(['Angela', 24, 'Data Scientist'])\nfile_content.writerow(['Julia', 24, 'Data Scientist'])\nfile_object.close()\n\n#Create a file named test.txt and save it in the current directory.\nfile_object = open('test.txt', 'w')\nfile_content = file_object.write('Hello World')\nfile_object.close()\n\n#Instantiate the RouteDomain class with a file named test.csv.\nroute_domain = RouteDomain('test.csv')\n#Print the file_entity attribute of the instance.\nprint(route_domain.file_entity)\n\n#Print the number of rows of the file.\nprint(route_domain.file_entity.read_csvfile())\n\n#Instantiate the RouteDomain class with a file named test.txt.\nroute_domain = RouteDomain('test.txt')\n#Print the file_entity attribute of the instance.\nprint(route_domain.file_entity)\n\n#Print the number of words of the file.\nprint(route_domain.file_entity.read_txtfile())\n\n#Instantiate the RouteDomain class with a file named test.pdf.\nroute_domain = RouteDomain('test.pdf')\n\n#Print the file_entity attribute of the instance.\nprint(route_domain.file_entity)\n\n#Print the file_extension attribute of the instance.\nprint(route_domain.file_extension)", '', "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        else:\n            print('File not supported')\n\nif __name__ == '__main__':\n    path = input('Type the name of the file: ')\n    route = RouteDomain(path)\n    route.file_entity.processing()\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_csv.csv\n\nfile_txt.txt\n\nfile_md.md\n\nfile_pdf.pdf\n\nfile_py.py\n\nfile_py.py\n\nfile_md.md\n\nfile_pdf.", "    def __init__(self, filepath):\n        self.file = filepath\n        self.extension = os.path.splitext(self.file)[1]\n        self.file_entity = None\n        if self.extension == '.csv':\n            self.file_entity = FileCSV(self.file)\n        else:\n            self.file_entity = FileTXT(self.file)\n            \n    def read_file(self):\n        return self.file_entity.read_file()\n    \n    def write_file(self, txt):\n        return self.file_entity.write_file(txt)\n        \n    def delete_file(self):\n        return self.file_entity.delete_file()\n\n#Use the RouteDomain class to read the file csv_file.csv.\n\nroute = RouteDomain('csv_file.csv')\nroute.read_file()\n\n#Use the RouteDomain class to read the file txt_file.txt.\n\nroute = RouteDomain('txt_file.txt')\nroute.read_file()\n\n#Use the RouteDomain class to delete the file csv_file.csv.\n\nroute = RouteDomain('csv_file.csv')\nroute.delete_file()\n\n#Use the RouteDomain class to delete the file txt_file.txt.\n\nroute = RouteDomain('txt_file.txt')\nroute.delete_file()\n\n#Use the RouteDomain class to write a new text in the file csv_file.csv.\n\nroute = RouteDomain('csv_file.csv')\nroute.write_file('Cristian')\n\n#Use the RouteDomain class to write a new text in the file txt_file.txt.\n\nroute = RouteDomain('txt_file.txt')\nroute.write_file('Cristian')", '', "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_extension = self.file.split('.')[-1]\n        \n    def get_file_extension(self):\n        return self.file_extension\n    \n    def get_file_entity(self):\n        if self.file_extension == 'csv':\n            return FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            return FileTXT(self.file)\n        else:\n            raise Exception('Unkown file extension')\n            \n \n\ncsv_domain = RouteDomain('data.csv')\n\ncsv_domain.get_file_extension()\n\ncsv_domain.get_file_entity()\n\ncsv_domain.get_file_entity().get_file_extension()\n\ntxt_domain = RouteDomain('data.txt')\n\ntxt_domain.get_file_extension()\n\ntxt_domain.get_file_entity()\n\ntxt_domain.get_file_entity().get_file_extension()\n \n\ntxt_domain = RouteDomain('data.txt')\n\ntxt_domain.get_file_extension()\n\ntxt_domain.get_file_entity()\n\ntxt_domain.get_file_entity().get_file_extension()\n\n\n\n# EXERCISE:\n\n# In this exercise you will create two classes, an abstract class and a concrete class. The abstract class is called Shape and it has two attributes called length and width. The concrete class is called Rectangle and it implements the area and perimeter functionality.\n\nclass Shape():\n    def __init__(self, length, width):\n        self.length = length\n        self.width = width\n        \n    def get_area(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n    def get_perimeter(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n        \nclass Rectangle(Shape):\n    def get_area(self):\n        return self.length * self.width\n    \n    def get_perimeter(self):\n        return 2 * self.length + 2 * self.width\n        \n        \nrectangle = Rectangle(2, 3)\n\nrectangle.get_area()\n\nrectangle.get_perimeter()\n \n\n# EXERCISE:\n\n# In this exercise you will create two classes, an abstract class and a concrete class. The abstract class is called Shape and it has two attributes called length and width. The concrete class is called Rectangle and it implements the area and perimeter functionality.\n\nclass Shape():\n    def __init__(self, length, width):\n        self.length = length\n        self.width = width\n        \n    def get_area(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n    def get_perimeter(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n        \nclass Rectangle(Shape):\n    def get_area(self):\n        return self.length * self.width\n    \n    def get_perimeter(self):\n        return 2 * self.length + 2 * self.width\n        \n        \nrectangle = Rectangle(2, 3)\n\nrectangle.get_area()\n\nrectangle.get_perimeter()\n \n\n# EXERCISE:\n\n# In this exercise you will create two classes, an abstract class and a concrete class. The abstract class is called Shape and it has two attributes called length and width. The concrete class is called Rectangle and it implements the area and perimeter functionality.\n\nclass Shape():\n    def __init__(self, length, width):\n        self.length = length\n        self.width = width\n        \n    def get_area(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n    def get_perimeter(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n        \nclass Rectangle(Shape):\n    def get_area(self):\n        return self.length * self.width\n    \n    def get_perimeter(self):\n        return 2 * self.length + 2 * self.width\n        \n        \nrectangle = Rectangle(2, 3)\n\nrectangle.get_area()\n\nrectangle.get_perimeter()\n \n\n# EXERCISE:\n\n# In this exercise you will create two classes, an abstract class and a concrete class. The abstract class is called Shape and it has two attributes called length and width. The concrete class is called Rectangle and it implements the area and perimeter functionality.\n\nclass Shape():\n    def __init__(self, length, width):\n        self.length = length\n        self.width = width\n        \n    def get_area(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n    def get_perimeter(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n        \nclass Rectangle(Shape):\n    def get_area(self):\n        return self.length * self.width\n    \n    def get_perimeter(self):\n        return 2 * self.length + 2 * self.width\n        \n        \nrectangle = Rectangle(2, 3)\n\nrectangle.get_area()\n\nrectangle.get_perimeter()\n \n\n# EXERCISE:\n\n# In this exercise you will create two classes, an abstract class and a concrete class. The abstract class is called Shape and it has two attributes called length and width. The concrete class is called Rectangle and it implements the area and perimeter functionality.\n\nclass Shape():\n    def __init__(self, length, width):\n        self.length = length\n        self.width = width\n        \n    def get_area(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n    def get_perimeter(self):\n        raise NotImplementedError('Subclass must implement abstract method')\n        \n        \nclass Rectangle(Shape):\n    def get_area(self):\n        return self.length * self.width\n    \n    def get_perimeter(self):\n        return 2 * self.length + 2 * self.width\n        \n        \nrectangle = Rectangle(2, 3)\n\nrectangle.get_area()\n\nrectangle", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n\nclass FileTXT():\n    def __init__(self, filepath):\n        self.file = filepath\n\nprint('\\n')\nprint('A class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.')\n\nprint('\\n')\nprint('File CSV')\nprint('\\n')\n\nprint(RouteDomain('file.csv').file_entity.file)\n\nprint('\\n')\nprint('File TXT')\nprint('\\n')\n\nprint(RouteDomain('file.txt').file_entity.file)\n\nprint('\\n')\nprint('\\n')\nprint('\\n')\nprint('\\n')\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n\nclass FileTXT():\n    def __init__(self, filepath):\n        self.file = filepath\n\nprint('\\n')\nprint('A class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.')\n\nprint('\\n')\nprint('File CSV')\nprint('\\n')\n\nprint(RouteDomain('file.csv').file_entity.file)\n\nprint('\\n')\nprint('File TXT')\nprint('\\n')\n\nprint(RouteDomain('file.txt').file_entity.file)\n\nprint('\\n')\nprint('\\n')\nprint('\\n')\nprint('\\n')\n\n#Return a class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.\n\nclass RouteDomain():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n\nclass FileTXT():\n    def __init__(self, filepath):\n        self.file = filepath\n\nprint('\\n')\nprint('A class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class.')\n\nprint('\\n')\nprint('File CSV')\nprint('\\n')\n\nprint(RouteDomain('file.csv').file_entity.file)\n\nprint('\\n')\nprint('File TXT')\nprint('\\n')\n\nprint(RouteDomain('file.txt').file_entity.file)\n\nprint('\\n')\nprint('\\n')\nprint('\\n')\nprint('\\n')", "    def __init__(self, filepath):\n        self.file = filepath\n        self.extension = self.file.split('.')[-1]\n        if self.extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        else:\n            print('The file has a not valid extension')\n            raise ValueError\n    def get_file_entity(self):\n        return self.file_entity\n&lt;/code&gt;\n", "    def __init__(self, filepath):\n        self.filepath = filepath\n        self.file = Path(filepath)\n        self.extension = self.file.suffix\n        if self.extension == '.csv':\n            self.file_entity = FileCSV(filepath)\n        else:\n            self.file_entity = FileTXT(filepath)\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.filepath = filepath\n        self.file = Path(filepath)\n        self.extension = self.file.suffix\n    def set_file_csv(self):\n        print(f'The file {self.file} is a csv')\n\nclass FileTXT():\n    def __init__(self, filepath):\n        self.filepath = filepath\n        self.file = Path(filepath)\n        self.extension = self.file.suffix\n    def set_file_txt(self):\n        print(f'The file {self.file} is a txt')\n&lt;/code&gt;\nWhen I run:\n&lt;code&gt;route = RouteDomain('file.csv')\nroute.file_entity.set_file_csv()\n\nroute = RouteDomain('file.txt')\nroute.file_entity.set_file_txt()\n&lt;/code&gt;\nI get the following output:\n&lt;code&gt;The file file.csv is a csv\nThe file file.txt is a txt\n&lt;/code&gt;\n", "\tdef __init__(self, filepath):\n\t\tself.file = filepath\n\t\tself.file_entity = None\n\t\tself.extension = self.file.split('.')[-1]\n\t\tif self.extension == 'csv':\n\t\t\tself.file_entity = FileCSV(self.file)\n\t\telif self.extension == 'txt':\n\t\t\tself.file_entity = FileTXT(self.file)\n\n#Return a class named FileCSV that inherits from FileDomain.\n\nclass FileCSV(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = csv.reader(self.file_entity)\n\t\tself.header = next(self.reader)\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range(0, self.columns):\n\t\t\tself.data[self.header[i]] = []\n\t\tfor row in self.reader:\n\t\t\tfor i in range(0, self.columns):\n\t\t\t\tself.data[self.header[i]].append(row[i])\n\n#Return a class named FileTXT that inherits from FileDomain.\n\nclass FileTXT(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = self.file_entity.read()\n\t\tself.header = self.reader.split('\\n')[0].split('\\t')\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range(0, self.columns):\n\t\t\tself.data[self.header[i]] = []\n\t\tfor row in self.reader.split('\\n')[1:]:\n\t\t\tfor i in range(0, self.columns):\n\t\t\t\tself.data[self.header[i]].append(row.split('\\t')[i])\n\n#Return a class named FileJSON that inherits from FileDomain.\n\nclass FileJSON(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = json.load(self.file_entity)\n\t\tself.header = list(self.reader.keys())\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range(0, self.columns):\n\t\t\tself.data[self.header[i]] = []\n\t\tfor row in range(0, len(self.reader[self.header[0]])):\n\t\t\tfor i in range(0, self.columns):\n\t\t\t\tself.data[self.header[i]].append(self.reader[self.header[i]][row])\n\n#Return a class named FileXML that inherits from FileDomain.\n\nclass FileXML(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = self.file_entity.read()\n\t\tself.root = ET.fromstring(self.reader)\n\t\tself.header = []\n\t\tfor items in self.root[0]:\n\t\t\tself.header.append(items.tag)\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range(0, self.columns):\n\t\t\tself.data[self.header[i]] = []\n\t\tfor row in self.root:\n\t\t\tfor i in range(0, self.columns):\n\t\t\t\tself.data[self.header[i]].append(row[i].text)\n\n#Return a class named FileHTML that inherits from FileDomain.\n\nclass FileHTML(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = self.file_entity.read()\n\t\tself.root = BeautifulSoup(self.reader, 'html.parser')\n\t\tself.header = []\n\t\tfor items in self.root.find_all('th'):\n\t\t\tself.header.append(items.text)\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range(0, self.columns):\n\t\t\tself.data[self.header[i]] = []\n\t\tfor row in self.root.find_all('tr'):\n\t\t\tfor i in range(0, self.columns):\n\t\t\t\tself.data[self.header[i]].append(row.find_all('td')[i].text)\n\n#Return a class named FilePDF that inherits from FileDomain.\n\nclass FilePDF(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = self.file_entity.read()\n\t\tself.data = {'text': []}\n\t\tfor page in PDFPage.get_pages(self.file_entity):\n\t\t\tinterpreter.process_page(page)\n\t\t\tself.data['text'].append(layout.get_text())\n\t\tself.header = ['text']\n\t\tself.columns = len(self.header)\n\n#Return a class named FileExcel that inherits from FileDomain.\n\nclass FileExcel(FileDomain):\n\tdef __init__(self, filepath):\n\t\tsuper().__init__(filepath)\n\t\tself.reader = self.file_entity.read()\n\t\tself.wb = xlrd.open_workbook(self.file)\n\t\tself.sheet = self.wb.sheet_by_index(0)\n\t\tself.header = []\n\t\tfor items in range(0, self.sheet.ncols):\n\t\t\tself.header.append(self.sheet.cell_value(0, items))\n\t\tself.columns = len(self.header)\n\t\tself.data = {}\n\t\tfor i in range"]</t>
+          <t>class RouteDomain()
+        def __init__(self, filepath):
+        self.file = filepath
+        ext = self.file.split('.')[-1]
+        self.file_entity = file_accepted[ext](self.file)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[False, False, False, False, False, False, True, False, False, False]</t>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>["    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.file_instance()\n    def file_instance(self):\n        # file_path = self.file\n        extension = self.file.split('.')[-1]\n        if extension == 'csv':\n            return FileCSV(self.file)\n        elif extension == 'txt':\n            return FileTXT(self.file)\n        else:\n            raise ValueError('Extension not allowed')\n\nclass FileCSV():\n    def __init__(self, file):\n        self.file = file\n    def read(self):\n        with open(self.file, 'r') as f:\n            return f.read()\n\n", '    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.extension = self.file.split(\'.\')[-1]\n        if self.extension == \'csv\':\n            self.file_entity = FileCSV(self.file)\n        elif self.extension == \'txt\':\n            self.file_entity = FileTXT(self.file)\n        else:\n            raise TypeError\n\nfrom route_domain import RouteDomain\n\nlogging.basicConfig(level=logging.INFO)\n\nif __name__ == \'__main__\':\n    path_data = \'route-views.routeviews.org_bgpdata_2019.06.txt\'\n    data = RouteDomain(path_data)\n    logging.info(data.file_entity.asn_as_prefix_dict)\n1562193600,1561932260,0.0.0.0/0,0,"2828 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12956",0,0.0.0.0,0,100,0,0,0,0,0,0,0\n1562193600,1561932260,1.0.0.0/24,7545,"7545 1299 12', "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_extension = self.file.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        else:\n            raise Exception('File type not supported')\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.file_name = self.file.split('/')[-1]\n        \n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.define_file_entity()\n    \n    def define_file_entity(self):\n        if self.file.endswith('.csv'):\n            self.file_entity = FileCSV(self.file)\n        elif self.file.endswith('.txt'):\n            self.file_entity = FileTXT(self.file)\n            \n    def get_file_entity(self):\n        return self.file_entity\nroute_domain = RouteDomain('../data/file.csv')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.txt')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xlsx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pdf')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.docx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.png')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.jpg')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.rar')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.gzip')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.gz')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.zip')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.json')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xml')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xls')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xlsb')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xlsx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xlt')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.xltx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.ods')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.dbf')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.db')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.sqlite')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.sqlite3')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.ppt')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptm')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity = route_domain.get_file_entity()\nfile_entity.read_file()\n\nroute_domain = RouteDomain('../data/file.pptx')\nfile_entity =", "    def __init__(self, filepath):\n        self.file = filepath\n        self.extension = self.file.split('.')[-1]\n        if self.extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        else:\n            self.file_entity = FileTXT(self.file)\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.extension = self.file.split('.')[-1]\n        if self.extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        else:\n            self.file_entity = FileTXT(self.file)\n            \n    def print_file(self):\n        print(self.file_entity.read_file())\n\nclass File(object):\n    def __init__(self, filepath):\n        self.filepath = filepath\n    \n    def read_file(self):\n        with open(self.filepath, 'r') as f:\n            return f.read()\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.extension = self.file.split('.')[-1]\n\n    def __getattr__(self, attr):\n        return getattr(self.file_entity, attr)\n\n    def __repr__(self):\n        return self.file_entity.__repr__()\n\n    def __str__(self):\n        return self.file_entity.__str__()\n\n    def __iter__(self):\n        return self.file_entity.__iter__()\n\n    def __next__(self):\n        return self.file_entity.__next__()\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.lines = None\n        self.read_file()\n\n    def read_file(self):\n        with open(self.file, 'r') as file:\n            self.lines = file.readlines()\n\n    def __repr__(self):\n        return 'FileCSV({})'.format(self.file)\n\n    def __str__(self):\n        return 'FileCSV: {}'.format(self.file)\n\n    def __iter__(self):\n        return iter(self.lines)\n\n    def __next__(self):\n        return next(self.lines)\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.create_entity()\n    \n    def create_entity(self):\n        if self.file.endswith('.csv'):\n            return FileCSV(self.file)\n        elif self.file.endswith('.txt'):\n            return FileTXT(self.file)\n        else:\n            return None\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.data = self.read_csv()\n    \n    def read_csv(self):\n        df = pd.read_csv(self.file)\n        return df\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.extension = self.file.split('.')[-1]\n        if self.extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        else:\n            self.file_entity = FileTXT(self.file)\n\nclass FileCSV():\n    def __init__(self, file):\n        self.file = file\n        self.number_of_lines = len(list(open(self.file)))\n\n", "    def __init__(self, filepath):\n        self.filepath = filepath\n        self.file = os.path.basename(filepath)\n        self.file_entity = self.file_entity()\n    def file_entity(self):\n        if self.file.split('.')[1] == 'csv':\n            file_entity = FileCSV(self.filepath)\n        elif self.file.split('.')[1] == 'txt':\n            file_entity = FileTXT(self.filepath)\n        return file_entity\n    \n    \n\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.filepath = filepath\n        self.file = os.path.basename(filepath)\n        self.df = self.read_csv()\n    def read_csv(self):\n        df = pd.read_csv(self.filepath)\n        return df.head()\n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n    \n\n"]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[True, False, True, False, True, True, False, True, True, False]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -526,7 +607,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Return a class named RouteDomain where an atributte called file is an input given to the class named filepath and obtain the extension of the file. Define a new attribute called file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class. Get each line of the file_entity and obtain a graph with it given a class called Graph. Store this in a new atribute named graph.</t>
+          <t>Define a class named RouteDomain that has an atributte called file. The attribute called file is equal to an input given to the class. The input given to the class is called filepath. Obtain the extension of the file. Define a new attribute in the class named file_entity that depending of the extension of the file instances a FileCSV class or a FileTXT class. Use a function called get_lines to read each line of the file_entity and store it in a variable called data.  Define a new attribute in the class named graph that using the variable data instances a Graph class. Do not use os or sys libraries</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -538,12 +619,43 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['', '', '', '', '', '', '', '', "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.get_file_entity()\n        self.graph = self.get_graph()\n\n    def get_file_entity(self):\n        filename, file_extension = os.path.splitext(self.file)\n        if file_extension == '.csv':\n            return FileCSV(self.file)\n        elif file_extension == '.txt':\n            return FileTXT(self.file)\n        else:\n            raise Exception('File format not allowed')\n\n    def get_graph(self):\n        graph = Graph()\n        for line in self.file_entity.get_lines():\n            graph.add_node(line[0])\n            graph.add_node(line[1])\n            graph.add_edge(line[0], line[1], int(line[2]))\n        return graph\n\n#Return a class named Route where an atributte named graph is a graph obtained by the class RouteDomain, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route that is a list of nodes from the start_node to the target_node.\n\nclass Route():\n    def __init__(self, filepath, start_node, target_node):\n        self.graph = RouteDomain(filepath).graph\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route = self.get_route()\n\n    def get_route(self):\n        route = []\n        if self.graph.is_connected(self.start_node, self.target_node):\n            route = self.graph.get_route(self.start_node, self.target_node)\n        return route\n\n#Define a class named RouteRun where an atributte named route is a route obtained by the class Route, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route.\n\nclass RouteRun():\n    def __init__(self, filepath, start_node, target_node):\n        self.route = Route(filepath, start_node, target_node).route\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = self.get_route_cost()\n\n    def get_route_cost(self):\n        route_cost = 0\n        if self.route:\n            route_cost = self.route[-1]['cost']\n        return route_cost\n\n#Define a class named RouteCost where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteCost():\n    def __init__(self, filepath, start_node, target_node):\n        self.file = filepath\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = RouteRun(self.file, self.start_node, self.target_node).route_cost\n\n#Define a class named RouteOptimizer where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteOptimizer():\n    def __init__(self, filepath, start_node, target_node):\n        self.file = filepath\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = RouteRun(self.file, self.start_node, self.target_node).route_cost\n\n#Define a class named RouteOptimizer where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteOptimizer():\n    def __init__(self, filepath, start_node, target_node):\n        self.file = filepath\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = RouteRun(self.file, self.start_node, self.target_node).route_cost\n\n#Define a class named RouteOptimizer where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteOptimizer():\n    def __init__(self, filepath, start_node, target_node):\n        self.file = filepath\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = RouteRun(self.file, self.start_node, self.target_node).route_cost\n\n#Define a class named RouteOptimizer where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteOptimizer():\n    def __init__(self, filepath, start_node, target_node):\n        self.file = filepath\n        self.start_node = start_node\n        self.target_node = target_node\n        self.route_cost = RouteRun(self.file, self.start_node, self.target_node).route_cost\n\n#Define a class named RouteOptimizer where an atributte named file is a string, an atributte named start_node is a string and an atributte named target_node is a string. Define a new atribute named route_cost that is the cost of the route obtained by the class RouteRun.\n\nclass RouteOptimizer():", '']</t>
+          <t>class RouteDomain()
+        def __init__(self, filepath):
+        self.file = filepath
+        ext = self.file.split('.')[-1]
+        self.file_entity = file_accepted[ext](self.file)
+        data = self.file_entity.get_lines()
+        self.graph = Graph(data)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[False, False, False, False, False, False, False, False, False, False]</t>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>["    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.graph = None\n        self.data = None\n        self.get_lines()\n        self.get_file_entity()\n        self.get_graph()\n        \n    def get_lines(self):\n        with open(self.file) as f:\n            self.data = f.readlines()\n            \n    def get_file_entity(self):\n        if self.file.endswith('.csv'):\n            self.file_entity = FileCSV(self.file)\n        elif self.file.endswith('.txt'):\n            self.file_entity = FileTXT(self.file)\n        else:\n            print('File not supported')\n            \n    def get_graph(self):\n        self.graph = Graph(self.data)\n\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.data = []\n        self.get_data()\n        \n    def get_data(self):\n        with open(self.file) as f:\n            self.data = f.readlines()\n\n\n", "\tdef __init__(self, filepath):\n\t\tself.file = filepath\n\t\ttry:\n\t\t\tself.file_entity = (FileCSV(self.file) if self.file.split('.')[1] == 'csv' else FileTXT(self.file))\n\t\t\tself.data = self.file_entity.get_lines()\n\t\t\tself.graph = Graph(self.data)\n\t\texcept Exception as e:\n\t\t\tprint(e)\n\n\nclass Graph():\n\tdef __init__(self, file_data):\n\t\tself.data = file_data\n\t\tself.g = {}\n\t\tfor line in self.data:\n\t\t\tself.g[line[0]] = [line[1:]]\n\t\tself.vertices = self.get_vertices()\n\t\tself.edges = self.get_edges()\n\n\tdef get_vertices(self):\n\t\treturn list(self.g.keys())\n\n\tdef get_edges(self):\n\t\treturn list(self.g.values())\n\n\tdef get_path(self, origin):\n\t\tself.origin = origin\n\t\treturn self.get_path_aux(self.origin, [])\n\n\tdef get_cost(self, origin):\n\t\tself.origin = origin\n\t\treturn self.get_cost_aux(self.origin, 0)\n\n\tdef get_time(self, origin):\n\t\tself.origin = origin\n\t\treturn self.get_time_aux(self.origin, 0)\n\n\tdef get_path_aux(self, origin, visited):\n\t\tself.origin = origin\n\t\tself.visited = visited\n\t\tself.visited.append(self.origin)\n\t\tfor edge in self.edges:\n\t\t\tif self.origin in edge[0]:\n\t\t\t\tfor vertex in edge[0]:\n\t\t\t\t\tif vertex not in self.visited:\n\t\t\t\t\t\tself.get_path_aux(vertex, self.visited)\n\t\treturn self.visited\n\n\tdef get_cost_aux(self, origin, cost):\n\t\tself.origin = origin\n\t\tself.cost = cost\n\t\tfor edge in self.edges:\n\t\t\tif self.origin in edge[0]:\n\t\t\t\tfor vertex in edge[0]:\n\t\t\t\t\tif vertex in self.visited:\n\t\t\t\t\t\tself.cost += int(edge[0][-1])\n\t\t\t\t\t\tself.get_cost_aux(vertex, self.cost)\n\t\treturn self.cost\n\n\tdef get_time_aux(self, origin, time):\n\t\tself.origin = origin\n\t\tself.time = time\n\t\tfor edge in self.edges:\n\t\t\tif self.origin in edge[0]:\n\t\t\t\tfor vertex in edge[0]:\n\t\t\t\t\tif vertex in self.visited:\n\t\t\t\t\t\tself.time += int(edge[0][-2])\n\t\t\t\t\t\tself.get_time_aux(vertex, self.time)\n\t\treturn self.time\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.graph = None\n        self.get_lines()\n        self.create_graph()\n    \n    def get_extension(self):\n        extension = self.file.split('.')[-1]\n        return extension\n    \n    def create_file_entity(self):\n        if self.get_extension() == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.get_extension() == 'txt':\n            self.file_entity = FileTXT(self.file)\n    \n    def get_lines(self):\n        self.create_file_entity()\n        data = self.file_entity.read_file()\n        return data\n    \n    def create_graph(self):\n        data = self.get_lines()\n        self.graph = Graph(data)\n\n\nclass File():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.read_file()\n        \n    def read_file(self):\n        with open(self.file, 'r') as file:\n            data = file.readlines()\n        data = [line.strip('\\n') for line in data]\n        return data\n    \n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = None\n        self.graph = None\n        self.get_lines()\n        self.create_graph()\n    \n    def get_lines(self):\n        file_extension = self.file.split('.')[-1]\n        if file_extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif file_extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        else:\n            print('Error')\n    \n    def create_graph(self):\n        self.graph = Graph(self.file_entity.data)\n\n\nclass FileCSV(File):\n    def read(self):\n        data = []\n        with open(self.file, 'r') as f:\n            reader = csv.reader(f)\n            for row in reader:\n                data.append(row)\n        self.data = data\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.extension = self.file.split('.')[-1]\n        if self.extension == 'csv':\n            self.file_entity = FileCSV(self.file)\n        elif self.extension == 'txt':\n            self.file_entity = FileTXT(self.file)\n        self.data = self.file_entity.get_lines()\n        self.graph = Graph(self.data)\n\n\nclass FileCSV(File):\n    def get_lines(self):\n        data = []\n        with open(self.file, 'r') as f:\n            reader = csv.reader(f)\n            for row in reader:\n                data.append(row)\n        return data\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.get_file_entity()\n        self.graph = self.get_graph()\n\n    def get_file_entity(self):\n        extension = self.file.split('.')[-1]\n        if extension == 'csv':\n            file_entity = FileCSV(self.file)\n        elif extension == 'txt':\n            file_entity = FileTXT(self.file)\n        return file_entity\n\n    def get_graph(self):\n        data = self.file_entity.get_lines()\n        graph = Graph(data)\n        return graph\n\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n\n    def get_lines(self):\n        with open(self.file, 'r') as f:\n            data = f.readlines()\n        return data\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.get_file_entity()\n        self.data = self.get_lines()\n        self.graph = self.create_graph()\n\n    def get_extension(self):\n        return self.file.split('.')[-1]\n\n    def get_file_entity(self):\n        if self.get_extension() == 'csv':\n            return FileCSV(self.file)\n        else:\n            return FileTXT(self.file)\n\n    def get_lines(self):\n        return self.file_entity.get_lines()\n\n    def create_graph(self):\n        return Graph(self.data)\n\n\nclass FileCSV():\n    def __init__(self, filepath):\n        self.file = filepath\n        self.lines = self.get_lines()\n\n    def get_lines(self):\n        with open(self.file, 'r') as file:\n            return [line.strip() for line in file.readlines()]\n\n\n", "\tdef __init__(self, filepath):\n\t\tself.file = filepath\n\t\tself.file_entity = self.file_entity()\n\t\tself.data = self.get_lines()\n\t\tself.graph = Graph(self.data)\n\n\tdef file_entity(self):\n\t\tif self.file.endswith('.csv'):\n\t\t\tfile_entity = FileCSV(self.file)\n\t\telif self.file.endswith('.txt'):\n\t\t\tfile_entity = FileTXT(self.file)\n\t\treturn file_entity\n\n\tdef get_lines(self):\n\t\treturn self.file_entity.read_lines()\n\n\tdef get_graph(self):\n\t\treturn self.graph\n\n\nclass FileCSV():\n\tdef __init__(self, filepath):\n\t\tself.file = filepath\n\n\tdef read_lines(self):\n\t\tdata = []\n\t\twith open(self.file, 'r') as f:\n\t\t\treader = csv.reader(f)\n\t\t\tfor line in reader:\n\t\t\t\tdata.append(line)\n\t\treturn data\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_entity = self.file_manager()\n        self.data = self.get_lines()\n        self.graph = Graph(self.data)\n\n    def file_manager(self):\n        extension = self.file.split('.')[-1]\n        if extension == 'csv':\n            return FileCSV(self.file)\n        elif extension == 'txt':\n            return FileTXT(self.file)\n\n    def get_lines(self):\n        data = self.file_entity.read()\n        return data\n\n\n\n\nclass Graph():\n    def __init__(self, data):\n        self.edges = self.graph_edges(data)\n\n    def graph_edges(self, data):\n        edges = []\n        for item in data:\n            edges.append((item[0], item[1], item[2]))\n        return edges\n\n\n\n", "    def __init__(self, filepath):\n        self.file = filepath\n        self.file_extension = filepath.split('.')[-1]\n        if self.file_extension == 'csv':\n            self.file_entity = FileCSV(filepath)\n        else:\n            self.file_entity = FileTXT(filepath)\n        self.data = self.file_entity.get_lines()\n        self.graph = Graph(self.data)\n\n    def find_shortest_path_between_two_vertices(self, origin, destiny):\n        return self.graph.find_shortest_path_between_two_vertices(origin, destiny)\n\n\n\n\n\n    def find_distance_between_two_vertices(self, origin, destiny):\n        return self.graph.find_distance_between_two_vertices(origin, destiny)\n\n    def find_number_of_trips_between_two_vertices(self, origin, destiny, maximum_stops):\n        return self.graph.find_number_of_trips_between_two_vertices(origin, destiny, maximum_stops)\n\n    def find_number_of_trips_between_two_vertices_with_exact_stops(self, origin, destiny, exact_stops):\n        return self.graph.find_number_of_trips_between_two_vertices_with_exact_stops(origin, destiny, exact_stops)\n\n    def find_length_of_shortest_route_between_two_vertices(self, origin, destiny, maximum_distance):\n        return self.graph.find_length_of_shortest_route_between_two_vertices(origin, destiny, maximum_distance)"]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[False, True, False, False, True, True, True, False, False, True]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>